<commit_message>
Wrapping up the code
</commit_message>
<xml_diff>
--- a/backend/app/vol/AT04 Inv.xlsx
+++ b/backend/app/vol/AT04 Inv.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jp65516\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Projects\AT-LRR\backend\app\vol\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4706,6 +4706,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4716,15 +4725,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5038,10 +5038,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="12"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="114"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="110"/>
     </row>
     <row r="3" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -14451,14 +14451,14 @@
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="108" t="s">
+      <c r="D1" s="111" t="s">
         <v>445</v>
       </c>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
-      <c r="I1" s="110"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="113"/>
     </row>
     <row r="2" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="90" t="s">
@@ -22355,13 +22355,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="40" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A154" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A161" sqref="A161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.42578125" style="19" customWidth="1"/>
+    <col min="1" max="1" width="56" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="82.28515625" style="26" customWidth="1"/>
     <col min="3" max="7" width="79.42578125" style="65" customWidth="1"/>
     <col min="8" max="8" width="62.28515625" style="65" customWidth="1"/>
@@ -22373,46 +22373,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="111" t="s">
+      <c r="B1" s="114" t="s">
         <v>519</v>
       </c>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111" t="s">
+      <c r="C1" s="114"/>
+      <c r="D1" s="114" t="s">
         <v>649</v>
       </c>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111" t="s">
+      <c r="E1" s="114"/>
+      <c r="F1" s="114" t="s">
         <v>738</v>
       </c>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111" t="s">
+      <c r="G1" s="114"/>
+      <c r="H1" s="114" t="s">
         <v>826</v>
       </c>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111" t="s">
+      <c r="I1" s="114"/>
+      <c r="J1" s="114" t="s">
         <v>902</v>
       </c>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111" t="s">
+      <c r="K1" s="114"/>
+      <c r="L1" s="114" t="s">
         <v>977</v>
       </c>
-      <c r="M1" s="111"/>
-      <c r="N1" s="111" t="s">
+      <c r="M1" s="114"/>
+      <c r="N1" s="114" t="s">
         <v>1069</v>
       </c>
-      <c r="O1" s="111"/>
-      <c r="P1" s="111" t="s">
+      <c r="O1" s="114"/>
+      <c r="P1" s="114" t="s">
         <v>1151</v>
       </c>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="111" t="s">
+      <c r="Q1" s="114"/>
+      <c r="R1" s="114" t="s">
         <v>1198</v>
       </c>
-      <c r="S1" s="111"/>
-      <c r="T1" s="111" t="s">
+      <c r="S1" s="114"/>
+      <c r="T1" s="114" t="s">
         <v>1212</v>
       </c>
-      <c r="U1" s="111"/>
+      <c r="U1" s="114"/>
       <c r="V1" s="107"/>
       <c r="W1" s="107"/>
       <c r="X1" s="107"/>
@@ -33869,16 +33869,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="23" orientation="portrait" r:id="rId1"/>
@@ -41224,11 +41224,11 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
+<XMLData TextToDisplay="RightsWATCHMark">13|CITI-PII-Internal|{00000000-0000-0000-0000-000000000000}</XMLData>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="RightsWATCHMark">13|CITI-PII-Internal|{00000000-0000-0000-0000-000000000000}</XMLData>
+<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -41238,13 +41238,13 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFAB1D30-0A66-47CD-8C26-1B7051C38452}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A43897C-EAAA-4C57-BE5F-74BC431F4181}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A43897C-EAAA-4C57-BE5F-74BC431F4181}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFAB1D30-0A66-47CD-8C26-1B7051C38452}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>